<commit_message>
adapted lesson to new galacticPubs workflow
</commit_message>
<xml_diff>
--- a/meta/version-info.xlsx
+++ b/meta/version-info.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>ver_num</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>Thanks to Emily Hudson (Nashville, TN) for suggestions.</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>Added classroom materials and remote fixes</t>
+  </si>
+  <si>
+    <t>First version with a full complement of in-person classroom versions of presentations and handouts. Fixed problem with Part 3 warm-up. The descriptions of the solution were backwards (i.e. the cipher is -3 encipher, +3 decipher, not the opposite).</t>
   </si>
   <si>
     <t>We use semantic versioning for lesson revision, just as software developers do.</t>
@@ -672,10 +681,18 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="A10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="17">
+        <v>44306.0</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="9"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -6660,31 +6677,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="22" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>